<commit_message>
Latest Update of RPA automation
</commit_message>
<xml_diff>
--- a/RPA_Automation/Playwright/amazon_products.xlsx
+++ b/RPA_Automation/Playwright/amazon_products.xlsx
@@ -468,7 +468,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Portronics Toad 23 Wireless Optical Mouse with 2.4GHz, USB Nano Dongle, Optical Orientation, Click Wheel, Adjustable DPI(Black)</t>
+          <t>Ambrane Wireless Mouse with 2.4GHz, USB Nano Dongle, Silent Click, Optical Orientation Click Wheel, 4 Buttons, 1600 Adjustable DPI, Both Hand Use, Compatible with PC, Mac, Laptop (Sliq 3, Black)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -478,7 +478,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4.0 out of 5 stars</t>
+          <t>3.8 out of 5 stars</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">

</xml_diff>